<commit_message>
inconsisten data third messsage...
</commit_message>
<xml_diff>
--- a/Calculators.xlsx
+++ b/Calculators.xlsx
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[0.20833, 0.416, 0.35566, 0.02001]</t>
+          <t>[0.34411, 0.25902, 0.30717, 0.08887]</t>
         </is>
       </c>
     </row>
@@ -471,12 +471,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[0.18353, 0.49734, 0.30161, 0.01752]</t>
+          <t>[0.34307, 0.29576, 0.26384, 0.09644]</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[0.16726, 0.53765, 0.27948, 0.0156]</t>
+          <t>[0.31417, 0.31515, 0.28813, 0.0818]</t>
         </is>
       </c>
     </row>
@@ -501,12 +501,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[0.32152, 0.20119, 0.45864, 0.01864]</t>
+          <t>[0.36434, 0.19005, 0.35467, 0.09012]</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[0.18313, 0.47322, 0.32552, 0.01813]</t>
+          <t>[0.32946, 0.2933, 0.29273, 0.08374]</t>
         </is>
       </c>
     </row>
@@ -531,12 +531,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[0.07333, 0.66474, 0.24614, 0.01579]</t>
+          <t>[0.31492, 0.31362, 0.28772, 0.08298]</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[0.29724, 0.24795, 0.43805, 0.01675]</t>
+          <t>[0.18489, 0.08773, 0.67646, 0.05005]</t>
         </is>
       </c>
     </row>
@@ -561,12 +561,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[0.06472, 0.77473, 0.15018, 0.01037]</t>
+          <t>[0.35593, 0.20305, 0.35293, 0.08722]</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[0.16171, 0.54534, 0.27645, 0.0165]</t>
+          <t>[0.01474, 0.97331, 0.00517, 0.00673]</t>
         </is>
       </c>
     </row>
@@ -591,12 +591,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[0.07762, 0.75147, 0.15934, 0.01158]</t>
+          <t>[0.33113, 0.25059, 0.33465, 0.08291]</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[0.05002, 0.81066, 0.13004, 0.00928]</t>
+          <t>[0.31677, 0.32805, 0.26937, 0.08505]</t>
         </is>
       </c>
     </row>
@@ -621,12 +621,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[0.15142, 0.57315, 0.25952, 0.01592]</t>
+          <t>[0.33358, 0.29303, 0.284, 0.0886]</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[0.39549, 0.05229, 0.51649, 0.03573]</t>
+          <t>[0.33253, 0.25418, 0.32771, 0.08484]</t>
         </is>
       </c>
     </row>
@@ -651,12 +651,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[0.06704, 0.76763, 0.15516, 0.01017]</t>
+          <t>[0.18907, 0.22605, 0.53388, 0.05027]</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[0.21585, 0.41743, 0.34962, 0.0171]</t>
+          <t>[0.34392, 0.26218, 0.30022, 0.09283]</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[0.40779, 0.12398, 0.45085, 0.01738]</t>
+          <t>[0.289, 0.26966, 0.37049, 0.07005]</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[0.12353, 0.62004, 0.24254, 0.01389]</t>
+          <t>[0.34617, 0.26262, 0.29926, 0.09112]</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[0.11943, 0.65105, 0.21521, 0.01431]</t>
+          <t>[0.15482, 0.40809, 0.39732, 0.03949]</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[0.32236, 0.10283, 0.55027, 0.02454]</t>
+          <t>[0.35264, 0.24113, 0.31505, 0.09036]</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[0.03022, 0.88359, 0.07932, 0.00687]</t>
+          <t>[0.32008, 0.36298, 0.23018, 0.08604]</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[0.11954, 0.65588, 0.21025, 0.01433]</t>
+          <t>[0.31607, 0.3057, 0.29313, 0.0843]</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[0.36272, 0.18313, 0.43718, 0.01697]</t>
+          <t>[0.2866, 0.2714, 0.36594, 0.0751]</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[0.281, 0.28017, 0.40931, 0.02952]</t>
+          <t>[0.31909, 0.28275, 0.31406, 0.08334]</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[0.47959, 0.06661, 0.41459, 0.03921]</t>
+          <t>[0.33853, 0.30124, 0.26792, 0.09145]</t>
         </is>
       </c>
     </row>
@@ -816,12 +816,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[0.17269, 0.50014, 0.31044, 0.01673]</t>
+          <t>[0.34063, 0.27321, 0.30149, 0.08387]</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[0.07961, 0.74725, 0.16172, 0.01143]</t>
+          <t>[0.3145, 0.31655, 0.28681, 0.08142]</t>
         </is>
       </c>
     </row>
@@ -846,12 +846,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[0.11953, 0.61921, 0.24612, 0.01513]</t>
+          <t>[0.32436, 0.31341, 0.27901, 0.08252]</t>
         </is>
       </c>
     </row>
@@ -861,12 +861,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[0.1481, 0.56379, 0.27124, 0.01688]</t>
+          <t>[0.33214, 0.25004, 0.33489, 0.08215]</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[0.16185, 0.52807, 0.29482, 0.01527]</t>
+          <t>[0.3694, 0.2569, 0.2832, 0.08969]</t>
         </is>
       </c>
     </row>
@@ -891,12 +891,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[0.11029, 0.63953, 0.23613, 0.01405]</t>
+          <t>[0.32003, 0.30275, 0.29376, 0.08272]</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[0.05413, 0.7953, 0.14081, 0.00976]</t>
+          <t>[0.33927, 0.28066, 0.28853, 0.09077]</t>
         </is>
       </c>
     </row>
@@ -921,12 +921,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[0.4167, 0.0431, 0.4988, 0.04141]</t>
+          <t>[0.3297, 0.30591, 0.27498, 0.08861]</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[0.05037, 0.82286, 0.11759, 0.00918]</t>
+          <t>[0.30565, 0.34162, 0.27058, 0.08145]</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[0.26785, 0.30629, 0.40596, 0.01989]</t>
+          <t>[0.31372, 0.22032, 0.383, 0.08203]</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[0.08368, 0.75, 0.15636, 0.00996]</t>
+          <t>[0.32999, 0.26199, 0.32646, 0.08075]</t>
         </is>
       </c>
     </row>
@@ -981,12 +981,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[0.13793, 0.58169, 0.26437, 0.01601]</t>
+          <t>[0.34317, 0.27309, 0.29269, 0.09022]</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[0.11793, 0.67982, 0.1892, 0.01305]</t>
+          <t>[0.17234, 0.25975, 0.52112, 0.04604]</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[0.07812, 0.75203, 0.15855, 0.0113]</t>
+          <t>[0.29843, 0.24874, 0.36541, 0.08653]</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[0.25754, 0.33303, 0.39083, 0.0186]</t>
+          <t>[0.3334, 0.28889, 0.29206, 0.08493]</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[0.0617, 0.7785, 0.14932, 0.01047]</t>
+          <t>[0.29792, 0.34844, 0.27516, 0.0778]</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[0.06433, 0.80046, 0.12647, 0.00874]</t>
+          <t>[0.29358, 0.32197, 0.3117, 0.07209]</t>
         </is>
       </c>
     </row>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[0.07886, 0.71761, 0.19139, 0.01214]</t>
+          <t>[0.34486, 0.21253, 0.35283, 0.08894]</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[0.21233, 0.3803, 0.38892, 0.01845]</t>
+          <t>[0.33047, 0.28539, 0.29573, 0.08765]</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1101,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[0.12081, 0.63901, 0.22585, 0.01433]</t>
+          <t>[0.33867, 0.2546, 0.32069, 0.08523]</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[0.14933, 0.58455, 0.25036, 0.01577]</t>
+          <t>[0.32258, 0.26303, 0.32814, 0.08547]</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[0.08846, 0.72592, 0.1736, 0.01202]</t>
+          <t>[0.15192, 0.42882, 0.32559, 0.09231]</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[0.2882, 0.29047, 0.40291, 0.01842]</t>
+          <t>[0.33637, 0.28348, 0.2958, 0.08359]</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[0.05544, 0.79952, 0.13521, 0.00983]</t>
+          <t>[0.29926, 0.28709, 0.34023, 0.07277]</t>
         </is>
       </c>
     </row>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[0.05671, 0.80763, 0.12627, 0.00939]</t>
+          <t>[0.15413, 0.15975, 0.65612, 0.02962]</t>
         </is>
       </c>
     </row>
@@ -1191,12 +1191,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>[0.2435, 0.35404, 0.38407, 0.01839]</t>
+          <t>[0.34167, 0.27586, 0.2946, 0.08706]</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[0.01881, 0.9298, 0.04627, 0.00512]</t>
+          <t>[0.29747, 0.35192, 0.27359, 0.07636]</t>
         </is>
       </c>
     </row>
@@ -1221,12 +1221,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[0.16466, 0.50898, 0.30974, 0.01662]</t>
+          <t>[0.33568, 0.27478, 0.29804, 0.09077]</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[0.098, 0.66201, 0.22574, 0.01425]</t>
+          <t>[0.30889, 0.3351, 0.27709, 0.07822]</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>[0.03032, 0.89276, 0.07119, 0.00572]</t>
+          <t>[0.16052, 0.40004, 0.3939, 0.04519]</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>[0.21239, 0.43049, 0.33817, 0.01895]</t>
+          <t>[0.22116, 0.58805, 0.10979, 0.08021]</t>
         </is>
       </c>
     </row>
@@ -1281,12 +1281,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>ideation</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[0.24352, 0.35078, 0.38803, 0.01766]</t>
+          <t>[0.32411, 0.34921, 0.24057, 0.0854]</t>
         </is>
       </c>
     </row>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[0.12459, 0.63562, 0.22647, 0.01332]</t>
+          <t>[0.32781, 0.27694, 0.31173, 0.08277]</t>
         </is>
       </c>
     </row>
@@ -1311,12 +1311,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>[0.11436, 0.64511, 0.22759, 0.01295]</t>
+          <t>[0.31488, 0.27763, 0.33217, 0.0746]</t>
         </is>
       </c>
     </row>
@@ -1326,12 +1326,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>ideation</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>[0.27746, 0.20006, 0.50401, 0.01847]</t>
+          <t>[0.30963, 0.3862, 0.22031, 0.08321]</t>
         </is>
       </c>
     </row>
@@ -1341,12 +1341,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>[0.15416, 0.51278, 0.31555, 0.01751]</t>
+          <t>[0.31066, 0.22949, 0.37754, 0.08141]</t>
         </is>
       </c>
     </row>
@@ -1356,12 +1356,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[0.29781, 0.23797, 0.44493, 0.01928]</t>
+          <t>[0.34583, 0.25326, 0.30918, 0.09086]</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[0.2784, 0.25112, 0.45251, 0.01797]</t>
+          <t>[0.3095, 0.2743, 0.33823, 0.07692]</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>ideation</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>[0.27729, 0.07148, 0.63082, 0.02042]</t>
+          <t>[0.29561, 0.36301, 0.26089, 0.07981]</t>
         </is>
       </c>
     </row>
@@ -1401,12 +1401,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>[0.08928, 0.69676, 0.2013, 0.01266]</t>
+          <t>[0.32858, 0.29108, 0.29201, 0.0876]</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>[0.0921, 0.68704, 0.20778, 0.01308]</t>
+          <t>[0.32548, 0.33549, 0.24619, 0.092]</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[0.09481, 0.69846, 0.19335, 0.01337]</t>
+          <t>[0.15365, 0.70187, 0.10222, 0.04177]</t>
         </is>
       </c>
     </row>
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[0.14033, 0.59326, 0.25023, 0.01618]</t>
+          <t>[0.34063, 0.23201, 0.33548, 0.09078]</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[0.10786, 0.71629, 0.16381, 0.01204]</t>
+          <t>[0.33261, 0.25811, 0.32203, 0.0864]</t>
         </is>
       </c>
     </row>
@@ -1476,12 +1476,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[0.13987, 0.56961, 0.27438, 0.01614]</t>
+          <t>[0.39262, 0.30209, 0.22619, 0.07852]</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[0.10033, 0.72062, 0.16638, 0.01267]</t>
+          <t>[0.01419, 0.96996, 0.00945, 0.00635]</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[0.23133, 0.39019, 0.35992, 0.01856]</t>
+          <t>[0.32557, 0.31705, 0.27049, 0.08619]</t>
         </is>
       </c>
     </row>
@@ -1521,12 +1521,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[0.19047, 0.53685, 0.25669, 0.01599]</t>
+          <t>[0.13455, 0.39697, 0.42331, 0.04472]</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>[0.04153, 0.856, 0.0951, 0.00738]</t>
+          <t>[0.01766, 0.97042, 0.00472, 0.00717]</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>[0.46228, 0.03913, 0.44705, 0.05153]</t>
+          <t>[0.31739, 0.30181, 0.29914, 0.08081]</t>
         </is>
       </c>
     </row>
@@ -1566,12 +1566,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>[0.31629, 0.21867, 0.44621, 0.01883]</t>
+          <t>[0.33332, 0.24735, 0.33168, 0.08682]</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[0.05587, 0.80489, 0.12986, 0.00938]</t>
+          <t>[0.31834, 0.32297, 0.27468, 0.08321]</t>
         </is>
       </c>
     </row>
@@ -1596,12 +1596,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[0.09665, 0.70703, 0.1834, 0.01292]</t>
+          <t>[0.34436, 0.22644, 0.33883, 0.0895]</t>
         </is>
       </c>
     </row>
@@ -1611,12 +1611,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>ideation</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>[0.33091, 0.17422, 0.47616, 0.01871]</t>
+          <t>[0.22495, 0.59292, 0.10428, 0.07731]</t>
         </is>
       </c>
     </row>
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>[0.22569, 0.3701, 0.38634, 0.01787]</t>
+          <t>[0.339, 0.28723, 0.28142, 0.0915]</t>
         </is>
       </c>
     </row>
@@ -1641,12 +1641,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>[0.14883, 0.58449, 0.25079, 0.01588]</t>
+          <t>[0.21215, 0.26748, 0.47715, 0.04265]</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>[0.08143, 0.74837, 0.15894, 0.01127]</t>
+          <t>[0.31772, 0.29092, 0.31086, 0.07972]</t>
         </is>
       </c>
     </row>
@@ -1671,12 +1671,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[0.08026, 0.72557, 0.18195, 0.01222]</t>
+          <t>[0.34542, 0.28628, 0.27667, 0.09082]</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1686,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>[0.11403, 0.64466, 0.22675, 0.01455]</t>
+          <t>[0.32729, 0.26165, 0.32844, 0.08185]</t>
         </is>
       </c>
     </row>
@@ -1701,12 +1701,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>[0.09289, 0.72096, 0.17501, 0.01114]</t>
+          <t>[0.32463, 0.27985, 0.31252, 0.08222]</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>[0.10244, 0.67137, 0.21258, 0.01361]</t>
+          <t>[0.34806, 0.28746, 0.26141, 0.10217]</t>
         </is>
       </c>
     </row>
@@ -1731,12 +1731,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[0.4558, 0.04255, 0.46609, 0.03556]</t>
+          <t>[0.33181, 0.2702, 0.31099, 0.08616]</t>
         </is>
       </c>
     </row>
@@ -1746,12 +1746,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[0.26922, 0.25026, 0.463, 0.01751]</t>
+          <t>[0.32797, 0.27302, 0.31141, 0.08676]</t>
         </is>
       </c>
     </row>
@@ -1761,12 +1761,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>[0.05258, 0.80962, 0.12806, 0.00974]</t>
+          <t>[0.32511, 0.2606, 0.332, 0.08153]</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>[0.5032, 0.02075, 0.44107, 0.03498]</t>
+          <t>[0.32787, 0.27416, 0.31291, 0.08428]</t>
         </is>
       </c>
     </row>
@@ -1791,12 +1791,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>[0.09755, 0.70558, 0.18386, 0.01301]</t>
+          <t>[0.3119, 0.30471, 0.30035, 0.08228]</t>
         </is>
       </c>
     </row>
@@ -1806,12 +1806,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>[0.08885, 0.71509, 0.18326, 0.0128]</t>
+          <t>[0.3453, 0.22336, 0.34771, 0.08258]</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>behavior</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[0.37317, 0.12826, 0.48043, 0.01815]</t>
+          <t>[0.36519, 0.21653, 0.31884, 0.09861]</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>[0.05987, 0.79696, 0.13326, 0.00992]</t>
+          <t>[0.31666, 0.32335, 0.27655, 0.08274]</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>[0.2706, 0.33404, 0.37752, 0.01784]</t>
+          <t>[0.18784, 0.34174, 0.42185, 0.0479]</t>
         </is>
       </c>
     </row>
@@ -1866,12 +1866,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>[0.14969, 0.55083, 0.2827, 0.01679]</t>
+          <t>[0.32696, 0.27842, 0.30849, 0.08534]</t>
         </is>
       </c>
     </row>
@@ -1881,12 +1881,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>[0.18425, 0.47515, 0.325, 0.01559]</t>
+          <t>[0.34581, 0.24275, 0.32474, 0.08589]</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ideation</t>
+          <t>indicator</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>[0.12563, 0.6057, 0.2529, 0.01577]</t>
+          <t>[0.35416, 0.25849, 0.29101, 0.09555]</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>[0.17787, 0.47053, 0.33485, 0.01675]</t>
+          <t>[0.30792, 0.32084, 0.28521, 0.08534]</t>
         </is>
       </c>
     </row>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>[0.02243, 0.90336, 0.06846, 0.00575]</t>
+          <t>[0.28982, 0.37505, 0.26472, 0.06981]</t>
         </is>
       </c>
     </row>
@@ -1941,12 +1941,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>indicator</t>
+          <t>behavior</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>[0.5108, 0.02045, 0.43646, 0.03229]</t>
+          <t>[0.1137, 0.30596, 0.55194, 0.02799]</t>
         </is>
       </c>
     </row>

</xml_diff>